<commit_message>
change to vite build optimize build package
add login

add import excel

finish StudentManagement
</commit_message>
<xml_diff>
--- a/public/temaplate.xlsx
+++ b/public/temaplate.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>FullName</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>1@gmail.com</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1224,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.72972972972973" defaultRowHeight="14.1" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1260,8 +1269,8 @@
       <c r="E2">
         <v>123456</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1280,8 +1289,8 @@
       <c r="E3">
         <v>123456</v>
       </c>
-      <c r="F3">
-        <v>1</v>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1300,8 +1309,8 @@
       <c r="E4">
         <v>123456</v>
       </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="F4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1320,8 +1329,8 @@
       <c r="E5">
         <v>123456</v>
       </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="F5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>